<commit_message>
Updates for feild testing
</commit_message>
<xml_diff>
--- a/XForms/Camping.xlsx
+++ b/XForms/Camping.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="78">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t xml:space="preserve">What is available ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">firepit</t>
   </si>
   <si>
     <t xml:space="preserve">minimal</t>
@@ -483,10 +486,10 @@
   <dimension ref="A1:AD15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="7:15"/>
+      <selection pane="topLeft" activeCell="F9" activeCellId="0" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.4765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.46875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.58"/>
@@ -695,63 +698,66 @@
       <c r="D8" s="12" t="s">
         <v>19</v>
       </c>
+      <c r="F8" s="12" t="s">
+        <v>20</v>
+      </c>
       <c r="I8" s="14" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" s="12" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="I9" s="14" t="s">
         <v>21</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="F9" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="I9" s="14" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="10" s="12" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="12" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B10" s="12" t="s">
         <v>1</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I10" s="14" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" s="13" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="13" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E11" s="10"/>
       <c r="F11" s="16"/>
       <c r="G11" s="16"/>
       <c r="H11" s="16"/>
       <c r="I11" s="13" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="K11" s="12"/>
       <c r="L11" s="17"/>
@@ -776,13 +782,13 @@
     </row>
     <row r="12" s="13" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="14" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D12" s="14"/>
       <c r="E12" s="18"/>
@@ -790,7 +796,7 @@
       <c r="G12" s="18"/>
       <c r="H12" s="18"/>
       <c r="I12" s="14" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J12" s="14"/>
       <c r="K12" s="12"/>
@@ -816,13 +822,13 @@
     </row>
     <row r="13" s="13" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="19" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C13" s="20" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D13" s="19"/>
       <c r="E13" s="21"/>
@@ -830,12 +836,12 @@
       <c r="G13" s="21"/>
       <c r="H13" s="21"/>
       <c r="I13" s="14" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J13" s="22"/>
       <c r="K13" s="12"/>
       <c r="L13" s="23" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="M13" s="17"/>
       <c r="N13" s="17"/>
@@ -858,13 +864,13 @@
     </row>
     <row r="14" s="13" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="19" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C14" s="20" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D14" s="19"/>
       <c r="E14" s="21"/>
@@ -872,12 +878,12 @@
       <c r="G14" s="21"/>
       <c r="H14" s="21"/>
       <c r="I14" s="14" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J14" s="22"/>
       <c r="K14" s="12"/>
       <c r="L14" s="23" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="M14" s="17"/>
       <c r="N14" s="17"/>
@@ -900,7 +906,7 @@
     </row>
     <row r="15" s="13" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="14" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B15" s="14"/>
       <c r="C15" s="14"/>
@@ -951,10 +957,10 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A16" activeCellId="1" sqref="7:15 A16"/>
+      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.4765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.46875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.82"/>
@@ -963,7 +969,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>1</v>
@@ -978,10 +984,10 @@
         <v>17</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -989,10 +995,10 @@
         <v>17</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1000,10 +1006,10 @@
         <v>17</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1011,10 +1017,10 @@
         <v>17</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1022,10 +1028,10 @@
         <v>17</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1033,10 +1039,10 @@
         <v>17</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1044,10 +1050,10 @@
         <v>17</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1055,10 +1061,10 @@
         <v>17</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1066,10 +1072,10 @@
         <v>17</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1077,10 +1083,10 @@
         <v>17</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1088,10 +1094,10 @@
         <v>17</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1099,10 +1105,10 @@
         <v>17</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1110,44 +1116,44 @@
         <v>17</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1169,10 +1175,10 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="7:15 A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.4765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.46875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1020" style="0" width="10.5"/>
@@ -1180,19 +1186,19 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="24" t="n">
         <f aca="true">NOW()</f>
-        <v>44391.4694842928</v>
+        <v>44451.8872291753</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>